<commit_message>
Removed relevance in evaluation metric
</commit_message>
<xml_diff>
--- a/Eval_scores.xlsx
+++ b/Eval_scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\65818\Documents\Computing notes of all types\mlops-assignment-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754A1890-BD91-4C71-A945-BD1A250EDD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B99136-2E04-42B0-8BCC-CA3ED9C7B9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C8A63716-432C-44AD-84C1-832839B18D5B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Query</t>
   </si>
@@ -93,56 +93,44 @@
     <t>Yes, SUTD offers a range of scholarships and financial aid options to support students' education. These include the SUTD Undergraduate Scholarship, the SUTD-MIT International Students Scholarship, and the SUTD-MIT International Students Loan. Additionally, SUTD provides financial aid to students who demonstrate financial need. The university also offers a range of other scholarships and awards, including the SUTD-MIT International Students Research Award and the SUTD-MIT International Students Capstone Project Award. These awards recognize students' academic achievements and provide financial support for their research and capstone projects. Overall, SUTD provides a range of financial aid options to support students' education and research."</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Same question ans answer as (1)</t>
+  </si>
+  <si>
+    <t>Faculty ratio is 1:11</t>
+  </si>
+  <si>
+    <t>Evaluation Score</t>
+  </si>
+  <si>
+    <t>Accuracy: 4/5
+Fluency: 5/5</t>
+  </si>
+  <si>
     <t>Accuracy: 2/5
-Relevance: 3/5
 Fluency: 5/5</t>
   </si>
   <si>
     <t>Accuracy: 2/5
-Relevance: 2/5
 Fluency: 4/5</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Same question ans answer as (1)</t>
-  </si>
-  <si>
-    <t>Accuracy: 4/5
-Relevance: 4/5
+    <t>Accuracy: 3/5
 Fluency: 5/5</t>
   </si>
   <si>
+    <t>Accuracy: 5/5
+Fluency: 5/5</t>
+  </si>
+  <si>
     <t>Accuracy: 2/5
-Relevance: 2/5
 Fluency: 3/5</t>
   </si>
   <si>
-    <t>Accuracy: 2/5
-Relevance: 2/5
-Fluency: 5/5</t>
-  </si>
-  <si>
-    <t>Accuracy: 3/5
-Relevance: 4/5
-Fluency: 5/5</t>
-  </si>
-  <si>
-    <t>Accuracy: 5/5
-Relevance: 5/5
-Fluency: 5/5</t>
-  </si>
-  <si>
-    <t>Faculty ratio is 1:11</t>
-  </si>
-  <si>
     <t>Accuracy: 1/5
-Relevance: 1/5
 Fluency: 3/5</t>
-  </si>
-  <si>
-    <t>Evaluation Score</t>
   </si>
 </sst>
 </file>
@@ -510,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57E5BD4-3015-432D-BC25-877883ABD839}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,10 +518,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -555,7 +543,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -569,7 +557,7 @@
         <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -580,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -591,7 +579,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -646,10 +634,10 @@
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="135" x14ac:dyDescent="0.25">

</xml_diff>